<commit_message>
Added new object productTagsEle in script and in xl sheet
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>productName</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>m-dfg</t>
+  </si>
+  <si>
+    <t>productTags</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
   </si>
 </sst>
 </file>
@@ -161,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -196,7 +211,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -405,20 +420,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -432,10 +447,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,10 +467,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -466,10 +487,13 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -483,10 +507,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -500,6 +527,9 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>